<commit_message>
update test page results
</commit_message>
<xml_diff>
--- a/pageTest/TestSheet-LuxiLiao.xlsx
+++ b/pageTest/TestSheet-LuxiLiao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DD21C5-2580-A04E-AB7C-3AA5927669B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94229F3-27CB-B543-BF97-87C9BCF5D5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" tabRatio="496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>Notes</t>
   </si>
@@ -336,12 +336,6 @@
     <t>spinner widget only shows valid values</t>
   </si>
   <si>
-    <t>A considerable number of style are not displayed correctly, inlcuding button and transparent effect. Some jQuery Validation messages are not correctly displayed as well (lacking style)</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>Most styles displayed, some have issue including background blending.</t>
   </si>
   <si>
@@ -390,23 +384,35 @@
     <t>Required Widgets are functional</t>
   </si>
   <si>
-    <t>Error Messages reflects input errors accurately.</t>
-  </si>
-  <si>
-    <t>IE does not correctly display validation messages correctly.</t>
-  </si>
-  <si>
     <t>test in Linux (Ubuntu 20.04)</t>
   </si>
   <si>
-    <t>User cannot submit form with missing data in required fields or invalid data</t>
+    <t>Error Messages should reflect input errors accurately.</t>
+  </si>
+  <si>
+    <t>User should not be able to submit form with missing data in required fields or invalid data</t>
+  </si>
+  <si>
+    <t>Page display should meet minimum viewable standard and allow user to properly read the page and intereact with it, on current platform.</t>
+  </si>
+  <si>
+    <t>Page display should meet minimum viewable standard and allow user to properly read the page and intereact with it.</t>
+  </si>
+  <si>
+    <t>A considerable number of style are not displayed correctly, inlcuding button and transparent effect. Some jQuery Validation messages are not correctly displayed as well (inappropriate style)</t>
+  </si>
+  <si>
+    <t>Effects like hovering does not work, unless with mouse connected</t>
+  </si>
+  <si>
+    <t>Effects like hovering does not work, even with mouse connected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +446,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -467,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -514,11 +526,163 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1240,10 +1404,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="162" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="119" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1357,12 +1521,16 @@
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="9"/>
+      <c r="E5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1439,16 +1607,14 @@
       <c r="F9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
@@ -1472,7 +1638,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1480,9 +1646,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="10"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="H11" s="14"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1530,11 +1694,15 @@
       <c r="C14" s="4"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="10"/>
+        <v>67</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1620,13 +1788,13 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>2</v>
@@ -1646,7 +1814,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>2</v>
@@ -1774,7 +1942,7 @@
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="144" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="128" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
@@ -1787,24 +1955,24 @@
       <c r="D28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="H28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1815,16 +1983,13 @@
       <c r="F29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="H29" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
@@ -1853,7 +2018,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="10" t="s">
@@ -1873,22 +2038,19 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H32" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
@@ -1897,7 +2059,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="10" t="s">
@@ -1928,18 +2090,20 @@
     </row>
     <row r="35" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="F35" s="10" t="s">
         <v>2</v>
       </c>
@@ -1947,12 +2111,7 @@
       <c r="H35" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
@@ -1961,7 +2120,7 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="10" t="s">
@@ -1974,18 +2133,20 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="H37" s="14" t="s">
         <v>28</v>
       </c>
@@ -1999,7 +2160,7 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="10" t="s">
@@ -2019,7 +2180,7 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="10" t="s">
@@ -2034,18 +2195,20 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="H40" s="14" t="s">
         <v>28</v>
       </c>
@@ -2138,129 +2301,245 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F46" s="17"/>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F47" s="17"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F48" s="17"/>
+      <c r="H48" s="14"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F49" s="17"/>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F50" s="17"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F51" s="17"/>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F53" s="17"/>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F54" s="17"/>
+      <c r="H54" s="14"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F55" s="17"/>
+      <c r="H55" s="14"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F56" s="17"/>
+      <c r="H56" s="14"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F57" s="17"/>
+      <c r="H57" s="14"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F58" s="17"/>
+      <c r="H58" s="14"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F59" s="17"/>
+      <c r="H59" s="14"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="18"/>
+      <c r="F61" s="17"/>
+      <c r="H61" s="14"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F62" s="17"/>
+      <c r="H62" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K10:K12 H2:H12 H18:H44">
-    <cfRule type="cellIs" dxfId="35" priority="30" operator="equal">
+  <conditionalFormatting sqref="K10:K12 H18:H44 H2:H12">
+    <cfRule type="cellIs" dxfId="50" priority="45" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="46" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="47" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K12 K18:K44">
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"Raised"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="49" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="50" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
       <formula>"Withdrawn"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H15">
-    <cfRule type="cellIs" dxfId="26" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="36" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K15">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="34" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"Raised"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
       <formula>"Withdrawn"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="27" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"Raised"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
       <formula>"Fixed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
       <formula>"Withdrawn"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="18" operator="equal">
       <formula>"Pending"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Issue"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"Raised"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+      <formula>"Fixed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+      <formula>"Withdrawn"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:H51">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53:H56">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57:H59">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H61">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"Raised"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
-      <formula>"Fixed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
-      <formula>"Withdrawn"</formula>
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H62">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>